<commit_message>
Adjusting Price importer TV data pull, problems with having start date too far in past, still needs fixing...
</commit_message>
<xml_diff>
--- a/Generic_Macro/SavedData/BTCUSD.xlsx
+++ b/Generic_Macro/SavedData/BTCUSD.xlsx
@@ -434,7 +434,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B4993"/>
+  <dimension ref="A1:B5031"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -40387,7 +40387,311 @@
         <v>45082</v>
       </c>
       <c r="B4993" t="n">
-        <v>27041.45</v>
+        <v>25732.88</v>
+      </c>
+    </row>
+    <row r="4994">
+      <c r="A4994" s="3" t="n">
+        <v>45083</v>
+      </c>
+      <c r="B4994" t="n">
+        <v>27238.18</v>
+      </c>
+    </row>
+    <row r="4995">
+      <c r="A4995" s="3" t="n">
+        <v>45084</v>
+      </c>
+      <c r="B4995" t="n">
+        <v>26351.68</v>
+      </c>
+    </row>
+    <row r="4996">
+      <c r="A4996" s="3" t="n">
+        <v>45085</v>
+      </c>
+      <c r="B4996" t="n">
+        <v>26512.76</v>
+      </c>
+    </row>
+    <row r="4997">
+      <c r="A4997" s="3" t="n">
+        <v>45086</v>
+      </c>
+      <c r="B4997" t="n">
+        <v>26488.23</v>
+      </c>
+    </row>
+    <row r="4998">
+      <c r="A4998" s="3" t="n">
+        <v>45087</v>
+      </c>
+      <c r="B4998" t="n">
+        <v>25858.78</v>
+      </c>
+    </row>
+    <row r="4999">
+      <c r="A4999" s="3" t="n">
+        <v>45088</v>
+      </c>
+      <c r="B4999" t="n">
+        <v>25940.01</v>
+      </c>
+    </row>
+    <row r="5000">
+      <c r="A5000" s="3" t="n">
+        <v>45089</v>
+      </c>
+      <c r="B5000" t="n">
+        <v>25912.41</v>
+      </c>
+    </row>
+    <row r="5001">
+      <c r="A5001" s="3" t="n">
+        <v>45090</v>
+      </c>
+      <c r="B5001" t="n">
+        <v>25936.28</v>
+      </c>
+    </row>
+    <row r="5002">
+      <c r="A5002" s="3" t="n">
+        <v>45091</v>
+      </c>
+      <c r="B5002" t="n">
+        <v>25130.06</v>
+      </c>
+    </row>
+    <row r="5003">
+      <c r="A5003" s="3" t="n">
+        <v>45092</v>
+      </c>
+      <c r="B5003" t="n">
+        <v>25582.77</v>
+      </c>
+    </row>
+    <row r="5004">
+      <c r="A5004" s="3" t="n">
+        <v>45093</v>
+      </c>
+      <c r="B5004" t="n">
+        <v>26336.15</v>
+      </c>
+    </row>
+    <row r="5005">
+      <c r="A5005" s="3" t="n">
+        <v>45094</v>
+      </c>
+      <c r="B5005" t="n">
+        <v>26515.09</v>
+      </c>
+    </row>
+    <row r="5006">
+      <c r="A5006" s="3" t="n">
+        <v>45095</v>
+      </c>
+      <c r="B5006" t="n">
+        <v>26342.29</v>
+      </c>
+    </row>
+    <row r="5007">
+      <c r="A5007" s="3" t="n">
+        <v>45096</v>
+      </c>
+      <c r="B5007" t="n">
+        <v>26844.45</v>
+      </c>
+    </row>
+    <row r="5008">
+      <c r="A5008" s="3" t="n">
+        <v>45097</v>
+      </c>
+      <c r="B5008" t="n">
+        <v>28317.58</v>
+      </c>
+    </row>
+    <row r="5009">
+      <c r="A5009" s="3" t="n">
+        <v>45098</v>
+      </c>
+      <c r="B5009" t="n">
+        <v>30002.77</v>
+      </c>
+    </row>
+    <row r="5010">
+      <c r="A5010" s="3" t="n">
+        <v>45099</v>
+      </c>
+      <c r="B5010" t="n">
+        <v>29898.58</v>
+      </c>
+    </row>
+    <row r="5011">
+      <c r="A5011" s="3" t="n">
+        <v>45100</v>
+      </c>
+      <c r="B5011" t="n">
+        <v>30705.83</v>
+      </c>
+    </row>
+    <row r="5012">
+      <c r="A5012" s="3" t="n">
+        <v>45101</v>
+      </c>
+      <c r="B5012" t="n">
+        <v>30548.39</v>
+      </c>
+    </row>
+    <row r="5013">
+      <c r="A5013" s="3" t="n">
+        <v>45102</v>
+      </c>
+      <c r="B5013" t="n">
+        <v>30473.14</v>
+      </c>
+    </row>
+    <row r="5014">
+      <c r="A5014" s="3" t="n">
+        <v>45103</v>
+      </c>
+      <c r="B5014" t="n">
+        <v>30274.34</v>
+      </c>
+    </row>
+    <row r="5015">
+      <c r="A5015" s="3" t="n">
+        <v>45104</v>
+      </c>
+      <c r="B5015" t="n">
+        <v>30700.05</v>
+      </c>
+    </row>
+    <row r="5016">
+      <c r="A5016" s="3" t="n">
+        <v>45105</v>
+      </c>
+      <c r="B5016" t="n">
+        <v>30083.26</v>
+      </c>
+    </row>
+    <row r="5017">
+      <c r="A5017" s="3" t="n">
+        <v>45106</v>
+      </c>
+      <c r="B5017" t="n">
+        <v>30453.02</v>
+      </c>
+    </row>
+    <row r="5018">
+      <c r="A5018" s="3" t="n">
+        <v>45107</v>
+      </c>
+      <c r="B5018" t="n">
+        <v>30477.68</v>
+      </c>
+    </row>
+    <row r="5019">
+      <c r="A5019" s="3" t="n">
+        <v>45108</v>
+      </c>
+      <c r="B5019" t="n">
+        <v>30594.48</v>
+      </c>
+    </row>
+    <row r="5020">
+      <c r="A5020" s="3" t="n">
+        <v>45109</v>
+      </c>
+      <c r="B5020" t="n">
+        <v>30625.3</v>
+      </c>
+    </row>
+    <row r="5021">
+      <c r="A5021" s="3" t="n">
+        <v>45110</v>
+      </c>
+      <c r="B5021" t="n">
+        <v>31160.43</v>
+      </c>
+    </row>
+    <row r="5022">
+      <c r="A5022" s="3" t="n">
+        <v>45111</v>
+      </c>
+      <c r="B5022" t="n">
+        <v>30776.54</v>
+      </c>
+    </row>
+    <row r="5023">
+      <c r="A5023" s="3" t="n">
+        <v>45112</v>
+      </c>
+      <c r="B5023" t="n">
+        <v>30507.27</v>
+      </c>
+    </row>
+    <row r="5024">
+      <c r="A5024" s="3" t="n">
+        <v>45113</v>
+      </c>
+      <c r="B5024" t="n">
+        <v>29911.02</v>
+      </c>
+    </row>
+    <row r="5025">
+      <c r="A5025" s="3" t="n">
+        <v>45114</v>
+      </c>
+      <c r="B5025" t="n">
+        <v>30352.3</v>
+      </c>
+    </row>
+    <row r="5026">
+      <c r="A5026" s="3" t="n">
+        <v>45115</v>
+      </c>
+      <c r="B5026" t="n">
+        <v>30299.25</v>
+      </c>
+    </row>
+    <row r="5027">
+      <c r="A5027" s="3" t="n">
+        <v>45116</v>
+      </c>
+      <c r="B5027" t="n">
+        <v>30174.62</v>
+      </c>
+    </row>
+    <row r="5028">
+      <c r="A5028" s="3" t="n">
+        <v>45117</v>
+      </c>
+      <c r="B5028" t="n">
+        <v>30423.95</v>
+      </c>
+    </row>
+    <row r="5029">
+      <c r="A5029" s="3" t="n">
+        <v>45118</v>
+      </c>
+      <c r="B5029" t="n">
+        <v>30631.36</v>
+      </c>
+    </row>
+    <row r="5030">
+      <c r="A5030" s="3" t="n">
+        <v>45119</v>
+      </c>
+      <c r="B5030" t="n">
+        <v>30396.78</v>
+      </c>
+    </row>
+    <row r="5031">
+      <c r="A5031" s="3" t="n">
+        <v>45120</v>
+      </c>
+      <c r="B5031" t="n">
+        <v>30555.37</v>
       </c>
     </row>
   </sheetData>
@@ -40401,7 +40705,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -40467,6 +40771,18 @@
         </is>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>Source</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>tv</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>